<commit_message>
Retrieved week 1 and final week queenless hive gcms files. Continued CHC identification in Br_Ib.
</commit_message>
<xml_diff>
--- a/data/raw/NM-recognition/tmp/Br_Ib_RT_ID_table.xlsx
+++ b/data/raw/NM-recognition/tmp/Br_Ib_RT_ID_table.xlsx
@@ -19,8 +19,32 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="K183" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Different compound</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="403">
   <si>
     <t xml:space="preserve">Peak</t>
   </si>
@@ -676,7 +700,7 @@
     <t xml:space="preserve">P168</t>
   </si>
   <si>
-    <t xml:space="preserve">C</t>
+    <t xml:space="preserve">C21_ene_NA</t>
   </si>
   <si>
     <t xml:space="preserve">P169</t>
@@ -694,6 +718,9 @@
     <t xml:space="preserve">P173</t>
   </si>
   <si>
+    <t xml:space="preserve">C21_ane_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P174</t>
   </si>
   <si>
@@ -721,6 +748,9 @@
     <t xml:space="preserve">P182</t>
   </si>
   <si>
+    <t xml:space="preserve">C22_ene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P183</t>
   </si>
   <si>
@@ -731,6 +761,9 @@
   </si>
   <si>
     <t xml:space="preserve">P186</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C22_ane_NA</t>
   </si>
   <si>
     <t xml:space="preserve">P187</t>
@@ -1253,12 +1286,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7B59"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1295,12 +1334,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1313,6 +1356,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF7B59"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1324,14 +1427,14 @@
   <dimension ref="A1:AQ350"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B169" activeCellId="0" sqref="B169"/>
+      <selection pane="bottomLeft" activeCell="D187" activeCellId="0" sqref="D187"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10347,7 +10450,9 @@
       <c r="A170" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B170" s="1"/>
+      <c r="B170" s="1" t="s">
+        <v>218</v>
+      </c>
       <c r="C170" s="1" t="n">
         <v>29.143775</v>
       </c>
@@ -10641,7 +10746,9 @@
       <c r="A174" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B174" s="1"/>
+      <c r="B174" s="1" t="s">
+        <v>224</v>
+      </c>
       <c r="C174" s="1" t="n">
         <v>29.54015</v>
       </c>
@@ -10768,7 +10875,7 @@
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B175" s="1"/>
       <c r="C175" s="1" t="n">
@@ -10819,7 +10926,7 @@
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B176" s="1"/>
       <c r="C176" s="1" t="n">
@@ -10876,7 +10983,7 @@
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B177" s="1"/>
       <c r="C177" s="1" t="n">
@@ -10966,7 +11073,7 @@
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B178" s="1"/>
       <c r="C178" s="1" t="n">
@@ -11041,7 +11148,7 @@
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B179" s="1"/>
       <c r="C179" s="1" t="n">
@@ -11167,7 +11274,7 @@
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B180" s="1"/>
       <c r="C180" s="1" t="n">
@@ -11188,7 +11295,7 @@
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B181" s="1"/>
       <c r="C181" s="1" t="n">
@@ -11236,7 +11343,7 @@
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B182" s="1"/>
       <c r="C182" s="1" t="n">
@@ -11266,9 +11373,11 @@
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="B183" s="1"/>
+        <v>233</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C183" s="1" t="n">
         <v>30.79515</v>
       </c>
@@ -11293,7 +11402,7 @@
       <c r="J183" s="1" t="n">
         <v>30.8</v>
       </c>
-      <c r="K183" s="1" t="n">
+      <c r="K183" s="2" t="n">
         <v>30.731</v>
       </c>
       <c r="L183" s="1" t="n">
@@ -11395,9 +11504,11 @@
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="B184" s="1"/>
+        <v>235</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="C184" s="1" t="n">
         <v>30.9145769230769</v>
       </c>
@@ -11482,7 +11593,7 @@
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B185" s="1"/>
       <c r="C185" s="1" t="n">
@@ -11500,7 +11611,7 @@
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B186" s="1"/>
       <c r="C186" s="1" t="n">
@@ -11578,9 +11689,11 @@
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B187" s="1"/>
+        <v>238</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>239</v>
+      </c>
       <c r="C187" s="1" t="n">
         <v>31.2747</v>
       </c>
@@ -11707,7 +11820,7 @@
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B188" s="1"/>
       <c r="C188" s="1" t="n">
@@ -11719,7 +11832,7 @@
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B189" s="1"/>
       <c r="C189" s="1" t="n">
@@ -11743,7 +11856,7 @@
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="1" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B190" s="1"/>
       <c r="C190" s="1" t="n">
@@ -11872,7 +11985,7 @@
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="1" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B191" s="1"/>
       <c r="C191" s="1" t="n">
@@ -11887,7 +12000,7 @@
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B192" s="1"/>
       <c r="C192" s="1" t="n">
@@ -11899,7 +12012,7 @@
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="1" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="B193" s="1"/>
       <c r="C193" s="1" t="n">
@@ -11938,7 +12051,7 @@
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="1" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="B194" s="1"/>
       <c r="C194" s="1" t="n">
@@ -11950,7 +12063,7 @@
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="1" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B195" s="1"/>
       <c r="C195" s="1" t="n">
@@ -12052,7 +12165,7 @@
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B196" s="1"/>
       <c r="C196" s="1" t="n">
@@ -12172,7 +12285,7 @@
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B197" s="1"/>
       <c r="C197" s="1" t="n">
@@ -12301,7 +12414,7 @@
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="1" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B198" s="1"/>
       <c r="C198" s="1" t="n">
@@ -12430,7 +12543,7 @@
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="1" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B199" s="1"/>
       <c r="C199" s="1" t="n">
@@ -12559,7 +12672,7 @@
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="1" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B200" s="1"/>
       <c r="C200" s="1" t="n">
@@ -12571,7 +12684,7 @@
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B201" s="1"/>
       <c r="C201" s="1" t="n">
@@ -12700,7 +12813,7 @@
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="1" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B202" s="1"/>
       <c r="C202" s="1" t="n">
@@ -12766,7 +12879,7 @@
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="1" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B203" s="1"/>
       <c r="C203" s="1" t="n">
@@ -12826,7 +12939,7 @@
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="1" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B204" s="1"/>
       <c r="C204" s="1" t="n">
@@ -12955,7 +13068,7 @@
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B205" s="1"/>
       <c r="C205" s="1" t="n">
@@ -13084,7 +13197,7 @@
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B206" s="1"/>
       <c r="C206" s="1" t="n">
@@ -13126,7 +13239,7 @@
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="1" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B207" s="1"/>
       <c r="C207" s="1" t="n">
@@ -13141,7 +13254,7 @@
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="1" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B208" s="1"/>
       <c r="C208" s="1" t="n">
@@ -13207,7 +13320,7 @@
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="1" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B209" s="1"/>
       <c r="C209" s="1" t="n">
@@ -13336,7 +13449,7 @@
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="1" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B210" s="1"/>
       <c r="C210" s="1" t="n">
@@ -13453,7 +13566,7 @@
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="1" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B211" s="1"/>
       <c r="C211" s="1" t="n">
@@ -13546,7 +13659,7 @@
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="1" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B212" s="1"/>
       <c r="C212" s="1" t="n">
@@ -13564,7 +13677,7 @@
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="1" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B213" s="1"/>
       <c r="C213" s="1" t="n">
@@ -13693,7 +13806,7 @@
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="1" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B214" s="1"/>
       <c r="C214" s="1" t="n">
@@ -13732,7 +13845,7 @@
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="1" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B215" s="1"/>
       <c r="C215" s="1" t="n">
@@ -13768,7 +13881,7 @@
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="1" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B216" s="1"/>
       <c r="C216" s="1" t="n">
@@ -13894,7 +14007,7 @@
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="1" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B217" s="1"/>
       <c r="C217" s="1" t="n">
@@ -13948,7 +14061,7 @@
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="1" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B218" s="1"/>
       <c r="C218" s="1" t="n">
@@ -14041,7 +14154,7 @@
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="1" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B219" s="1"/>
       <c r="C219" s="1" t="n">
@@ -14098,7 +14211,7 @@
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="1" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B220" s="1"/>
       <c r="C220" s="1" t="n">
@@ -14161,7 +14274,7 @@
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="1" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B221" s="1"/>
       <c r="C221" s="1" t="n">
@@ -14173,7 +14286,7 @@
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="1" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B222" s="1"/>
       <c r="C222" s="1" t="n">
@@ -14302,7 +14415,7 @@
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="1" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B223" s="1"/>
       <c r="C223" s="1" t="n">
@@ -14431,7 +14544,7 @@
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="1" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="B224" s="1"/>
       <c r="C224" s="1" t="n">
@@ -14461,7 +14574,7 @@
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B225" s="1"/>
       <c r="C225" s="1" t="n">
@@ -14590,7 +14703,7 @@
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B226" s="1"/>
       <c r="C226" s="1" t="n">
@@ -14677,7 +14790,7 @@
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="1" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B227" s="1"/>
       <c r="C227" s="1" t="n">
@@ -14806,7 +14919,7 @@
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="1" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="B228" s="1"/>
       <c r="C228" s="1" t="n">
@@ -14932,7 +15045,7 @@
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="1" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B229" s="1"/>
       <c r="C229" s="1" t="n">
@@ -14944,7 +15057,7 @@
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="1" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B230" s="1"/>
       <c r="C230" s="1" t="n">
@@ -15019,7 +15132,7 @@
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="1" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B231" s="1"/>
       <c r="C231" s="1" t="n">
@@ -15106,7 +15219,7 @@
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="1" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B232" s="1"/>
       <c r="C232" s="1" t="n">
@@ -15235,7 +15348,7 @@
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="1" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="B233" s="1"/>
       <c r="C233" s="1" t="n">
@@ -15250,7 +15363,7 @@
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="1" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="B234" s="1"/>
       <c r="C234" s="1" t="n">
@@ -15379,7 +15492,7 @@
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="1" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B235" s="1"/>
       <c r="C235" s="1" t="n">
@@ -15403,7 +15516,7 @@
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="1" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B236" s="1"/>
       <c r="C236" s="1" t="n">
@@ -15415,7 +15528,7 @@
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="1" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="B237" s="1"/>
       <c r="C237" s="1" t="n">
@@ -15538,7 +15651,7 @@
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="1" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B238" s="1"/>
       <c r="C238" s="1" t="n">
@@ -15640,7 +15753,7 @@
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="1" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="B239" s="1"/>
       <c r="C239" s="1" t="n">
@@ -15736,7 +15849,7 @@
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="1" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="B240" s="1"/>
       <c r="C240" s="1" t="n">
@@ -15850,7 +15963,7 @@
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="1" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B241" s="1"/>
       <c r="C241" s="1" t="n">
@@ -15979,7 +16092,7 @@
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="1" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="B242" s="1"/>
       <c r="C242" s="1" t="n">
@@ -16108,7 +16221,7 @@
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="1" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B243" s="1"/>
       <c r="C243" s="1" t="n">
@@ -16138,7 +16251,7 @@
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="1" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B244" s="1"/>
       <c r="C244" s="1" t="n">
@@ -16267,7 +16380,7 @@
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="1" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B245" s="1"/>
       <c r="C245" s="1" t="n">
@@ -16306,7 +16419,7 @@
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="1" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="B246" s="1"/>
       <c r="C246" s="1" t="n">
@@ -16435,7 +16548,7 @@
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="1" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B247" s="1"/>
       <c r="C247" s="1" t="n">
@@ -16447,7 +16560,7 @@
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="1" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="B248" s="1"/>
       <c r="C248" s="1" t="n">
@@ -16528,7 +16641,7 @@
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="1" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="B249" s="1"/>
       <c r="C249" s="1" t="n">
@@ -16549,7 +16662,7 @@
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="1" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="B250" s="1"/>
       <c r="C250" s="1" t="n">
@@ -16627,7 +16740,7 @@
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="1" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B251" s="1"/>
       <c r="C251" s="1" t="n">
@@ -16657,7 +16770,7 @@
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="1" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B252" s="1"/>
       <c r="C252" s="1" t="n">
@@ -16786,7 +16899,7 @@
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="1" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="B253" s="1"/>
       <c r="C253" s="1" t="n">
@@ -16810,7 +16923,7 @@
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="1" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="B254" s="1"/>
       <c r="C254" s="1" t="n">
@@ -16939,7 +17052,7 @@
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="1" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="B255" s="1"/>
       <c r="C255" s="1" t="n">
@@ -16951,7 +17064,7 @@
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="1" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="B256" s="1"/>
       <c r="C256" s="1" t="n">
@@ -16978,7 +17091,7 @@
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="1" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="B257" s="1"/>
       <c r="C257" s="1" t="n">
@@ -17107,7 +17220,7 @@
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="1" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B258" s="1"/>
       <c r="C258" s="1" t="n">
@@ -17125,7 +17238,7 @@
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="1" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="B259" s="1"/>
       <c r="C259" s="1" t="n">
@@ -17251,7 +17364,7 @@
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="1" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="B260" s="1"/>
       <c r="C260" s="1" t="n">
@@ -17335,7 +17448,7 @@
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="1" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="B261" s="1"/>
       <c r="C261" s="1" t="n">
@@ -17422,7 +17535,7 @@
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="1" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="B262" s="1"/>
       <c r="C262" s="1" t="n">
@@ -17500,7 +17613,7 @@
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="1" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="B263" s="1"/>
       <c r="C263" s="1" t="n">
@@ -17617,7 +17730,7 @@
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="1" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="B264" s="1"/>
       <c r="C264" s="1" t="n">
@@ -17629,7 +17742,7 @@
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="1" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="B265" s="1"/>
       <c r="C265" s="1" t="n">
@@ -17758,7 +17871,7 @@
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="1" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="B266" s="1"/>
       <c r="C266" s="1" t="n">
@@ -17824,7 +17937,7 @@
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="1" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="B267" s="1"/>
       <c r="C267" s="1" t="n">
@@ -17953,7 +18066,7 @@
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="1" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="B268" s="1"/>
       <c r="C268" s="1" t="n">
@@ -17974,7 +18087,7 @@
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="1" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="B269" s="1"/>
       <c r="C269" s="1" t="n">
@@ -18064,7 +18177,7 @@
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="1" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="B270" s="1"/>
       <c r="C270" s="1" t="n">
@@ -18181,7 +18294,7 @@
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="1" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="B271" s="1"/>
       <c r="C271" s="1" t="n">
@@ -18220,7 +18333,7 @@
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="1" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="B272" s="1"/>
       <c r="C272" s="1" t="n">
@@ -18337,7 +18450,7 @@
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="1" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="B273" s="1"/>
       <c r="C273" s="1" t="n">
@@ -18412,7 +18525,7 @@
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="1" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="B274" s="1"/>
       <c r="C274" s="1" t="n">
@@ -18520,7 +18633,7 @@
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="1" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="B275" s="1"/>
       <c r="C275" s="1" t="n">
@@ -18532,7 +18645,7 @@
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="1" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="B276" s="1"/>
       <c r="C276" s="1" t="n">
@@ -18604,7 +18717,7 @@
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="1" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="B277" s="1"/>
       <c r="C277" s="1" t="n">
@@ -18685,7 +18798,7 @@
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="1" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="B278" s="1"/>
       <c r="C278" s="1" t="n">
@@ -18697,7 +18810,7 @@
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="1" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="B279" s="1"/>
       <c r="C279" s="1" t="n">
@@ -18766,7 +18879,7 @@
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="1" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="B280" s="1"/>
       <c r="C280" s="1" t="n">
@@ -18895,7 +19008,7 @@
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="1" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="B281" s="1"/>
       <c r="C281" s="1" t="n">
@@ -19024,7 +19137,7 @@
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="1" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="B282" s="1"/>
       <c r="C282" s="1" t="n">
@@ -19153,7 +19266,7 @@
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="1" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="B283" s="1"/>
       <c r="C283" s="1" t="n">
@@ -19183,7 +19296,7 @@
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="1" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="B284" s="1"/>
       <c r="C284" s="1" t="n">
@@ -19312,7 +19425,7 @@
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="1" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="B285" s="1"/>
       <c r="C285" s="1" t="n">
@@ -19327,7 +19440,7 @@
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="1" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="B286" s="1"/>
       <c r="C286" s="1" t="n">
@@ -19450,7 +19563,7 @@
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="1" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="B287" s="1"/>
       <c r="C287" s="1" t="n">
@@ -19501,7 +19614,7 @@
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="1" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="B288" s="1"/>
       <c r="C288" s="1" t="n">
@@ -19561,7 +19674,7 @@
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="1" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="B289" s="1"/>
       <c r="C289" s="1" t="n">
@@ -19627,7 +19740,7 @@
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="1" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="B290" s="1"/>
       <c r="C290" s="1" t="n">
@@ -19726,7 +19839,7 @@
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="1" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="B291" s="1"/>
       <c r="C291" s="1" t="n">
@@ -19738,7 +19851,7 @@
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="1" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="B292" s="1"/>
       <c r="C292" s="1" t="n">
@@ -19789,7 +19902,7 @@
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="1" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="B293" s="1"/>
       <c r="C293" s="1" t="n">
@@ -19915,7 +20028,7 @@
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="B294" s="1"/>
       <c r="C294" s="1" t="n">
@@ -20014,7 +20127,7 @@
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="1" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="B295" s="1"/>
       <c r="C295" s="1" t="n">
@@ -20062,7 +20175,7 @@
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="1" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="B296" s="1"/>
       <c r="C296" s="1" t="n">
@@ -20092,7 +20205,7 @@
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="1" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="B297" s="1"/>
       <c r="C297" s="1" t="n">
@@ -20221,7 +20334,7 @@
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="1" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="B298" s="1"/>
       <c r="C298" s="1" t="n">
@@ -20350,7 +20463,7 @@
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="1" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B299" s="1"/>
       <c r="C299" s="1" t="n">
@@ -20407,7 +20520,7 @@
     </row>
     <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="1" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="B300" s="1"/>
       <c r="C300" s="1" t="n">
@@ -20518,7 +20631,7 @@
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="1" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B301" s="1"/>
       <c r="C301" s="1" t="n">
@@ -20533,7 +20646,7 @@
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="1" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B302" s="1"/>
       <c r="C302" s="1" t="n">
@@ -20662,7 +20775,7 @@
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="1" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B303" s="1"/>
       <c r="C303" s="1" t="n">
@@ -20695,7 +20808,7 @@
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="1" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B304" s="1"/>
       <c r="C304" s="1" t="n">
@@ -20824,7 +20937,7 @@
     </row>
     <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="1" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B305" s="1"/>
       <c r="C305" s="1" t="n">
@@ -20857,7 +20970,7 @@
     </row>
     <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="1" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B306" s="1"/>
       <c r="C306" s="1" t="n">
@@ -20932,7 +21045,7 @@
     </row>
     <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="1" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B307" s="1"/>
       <c r="C307" s="1" t="n">
@@ -21028,7 +21141,7 @@
     </row>
     <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="1" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="B308" s="1"/>
       <c r="C308" s="1" t="n">
@@ -21100,7 +21213,7 @@
     </row>
     <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="1" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="B309" s="1"/>
       <c r="C309" s="1" t="n">
@@ -21208,7 +21321,7 @@
     </row>
     <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="1" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="B310" s="1"/>
       <c r="C310" s="1" t="n">
@@ -21244,7 +21357,7 @@
     </row>
     <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="1" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="B311" s="1"/>
       <c r="C311" s="1" t="n">
@@ -21292,7 +21405,7 @@
     </row>
     <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="1" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="B312" s="1"/>
       <c r="C312" s="1" t="n">
@@ -21307,7 +21420,7 @@
     </row>
     <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B313" s="1"/>
       <c r="C313" s="1" t="n">
@@ -21322,7 +21435,7 @@
     </row>
     <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="1" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="B314" s="1"/>
       <c r="C314" s="1" t="n">
@@ -21448,7 +21561,7 @@
     </row>
     <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="1" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="B315" s="1"/>
       <c r="C315" s="1" t="n">
@@ -21511,7 +21624,7 @@
     </row>
     <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="1" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="B316" s="1"/>
       <c r="C316" s="1" t="n">
@@ -21598,7 +21711,7 @@
     </row>
     <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="1" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="B317" s="1"/>
       <c r="C317" s="1" t="n">
@@ -21661,7 +21774,7 @@
     </row>
     <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="1" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="B318" s="1"/>
       <c r="C318" s="1" t="n">
@@ -21784,7 +21897,7 @@
     </row>
     <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="1" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="B319" s="1"/>
       <c r="C319" s="1" t="n">
@@ -21796,7 +21909,7 @@
     </row>
     <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="1" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="B320" s="1"/>
       <c r="C320" s="1" t="n">
@@ -21808,7 +21921,7 @@
     </row>
     <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="B321" s="1"/>
       <c r="C321" s="1" t="n">
@@ -21850,7 +21963,7 @@
     </row>
     <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="B322" s="1"/>
       <c r="C322" s="1" t="n">
@@ -21871,7 +21984,7 @@
     </row>
     <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="1" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="B323" s="1"/>
       <c r="C323" s="1" t="n">
@@ -21901,7 +22014,7 @@
     </row>
     <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="1" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="B324" s="1"/>
       <c r="C324" s="1" t="n">
@@ -21991,7 +22104,7 @@
     </row>
     <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="B325" s="1"/>
       <c r="C325" s="1" t="n">
@@ -22045,7 +22158,7 @@
     </row>
     <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="1" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="B326" s="1"/>
       <c r="C326" s="1" t="n">
@@ -22102,7 +22215,7 @@
     </row>
     <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="1" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="B327" s="1"/>
       <c r="C327" s="1" t="n">
@@ -22117,7 +22230,7 @@
     </row>
     <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="1" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="B328" s="1"/>
       <c r="C328" s="1" t="n">
@@ -22222,7 +22335,7 @@
     </row>
     <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="1" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="B329" s="1"/>
       <c r="C329" s="1" t="n">
@@ -22324,7 +22437,7 @@
     </row>
     <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="1" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="B330" s="1"/>
       <c r="C330" s="1" t="n">
@@ -22336,7 +22449,7 @@
     </row>
     <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="1" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="B331" s="1"/>
       <c r="C331" s="1" t="n">
@@ -22348,7 +22461,7 @@
     </row>
     <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="1" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="B332" s="1"/>
       <c r="C332" s="1" t="n">
@@ -22423,7 +22536,7 @@
     </row>
     <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="1" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="B333" s="1"/>
       <c r="C333" s="1" t="n">
@@ -22435,7 +22548,7 @@
     </row>
     <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="1" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="B334" s="1"/>
       <c r="C334" s="1" t="n">
@@ -22450,7 +22563,7 @@
     </row>
     <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="1" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="B335" s="1"/>
       <c r="C335" s="1" t="n">
@@ -22468,7 +22581,7 @@
     </row>
     <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="1" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="B336" s="1"/>
       <c r="C336" s="1" t="n">
@@ -22597,7 +22710,7 @@
     </row>
     <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="1" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="B337" s="1"/>
       <c r="C337" s="1" t="n">
@@ -22621,7 +22734,7 @@
     </row>
     <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="1" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="B338" s="1"/>
       <c r="C338" s="1" t="n">
@@ -22696,7 +22809,7 @@
     </row>
     <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="1" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="B339" s="1"/>
       <c r="C339" s="1" t="n">
@@ -22741,7 +22854,7 @@
     </row>
     <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="1" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="B340" s="1"/>
       <c r="C340" s="1" t="n">
@@ -22753,7 +22866,7 @@
     </row>
     <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="1" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="B341" s="1"/>
       <c r="C341" s="1" t="n">
@@ -22804,7 +22917,7 @@
     </row>
     <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="1" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="B342" s="1"/>
       <c r="C342" s="1" t="n">
@@ -22819,7 +22932,7 @@
     </row>
     <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="1" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="B343" s="1"/>
       <c r="C343" s="1" t="n">
@@ -22846,7 +22959,7 @@
     </row>
     <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="B344" s="1"/>
       <c r="C344" s="1" t="n">
@@ -22861,7 +22974,7 @@
     </row>
     <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="1" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="B345" s="1"/>
       <c r="C345" s="1" t="n">
@@ -22933,7 +23046,7 @@
     </row>
     <row r="346" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="1" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="B346" s="1"/>
       <c r="C346" s="1" t="n">
@@ -23062,7 +23175,7 @@
     </row>
     <row r="347" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="1" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="B347" s="1"/>
       <c r="C347" s="1" t="n">
@@ -23128,7 +23241,7 @@
     </row>
     <row r="348" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="1" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="B348" s="1"/>
       <c r="C348" s="1" t="n">
@@ -23143,7 +23256,7 @@
     </row>
     <row r="349" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="1" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="B349" s="1"/>
       <c r="C349" s="1" t="n">
@@ -23155,7 +23268,7 @@
     </row>
     <row r="350" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="1" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="B350" s="1"/>
       <c r="C350" s="1" t="n">
@@ -23176,5 +23289,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Continued CHC identification for Br Ib.
</commit_message>
<xml_diff>
--- a/data/raw/NM-recognition/tmp/Br_Ib_RT_ID_table.xlsx
+++ b/data/raw/NM-recognition/tmp/Br_Ib_RT_ID_table.xlsx
@@ -39,12 +39,54 @@
         </r>
       </text>
     </comment>
+    <comment ref="K196" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Different compound</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T286" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Overlapped with another compound</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W272" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Might be different compound </t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="425">
   <si>
     <t xml:space="preserve">Peak</t>
   </si>
@@ -793,9 +835,15 @@
     <t xml:space="preserve">P195</t>
   </si>
   <si>
+    <t xml:space="preserve">C23_diene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P196</t>
   </si>
   <si>
+    <t xml:space="preserve">C23_ene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P197</t>
   </si>
   <si>
@@ -808,6 +856,9 @@
     <t xml:space="preserve">P200</t>
   </si>
   <si>
+    <t xml:space="preserve">C23_ane_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P201</t>
   </si>
   <si>
@@ -832,6 +883,9 @@
     <t xml:space="preserve">P208</t>
   </si>
   <si>
+    <t xml:space="preserve">C24_ene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P209</t>
   </si>
   <si>
@@ -844,6 +898,9 @@
     <t xml:space="preserve">P212</t>
   </si>
   <si>
+    <t xml:space="preserve">C24_ane_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P213</t>
   </si>
   <si>
@@ -871,6 +928,9 @@
     <t xml:space="preserve">P221</t>
   </si>
   <si>
+    <t xml:space="preserve">C25_ene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P222</t>
   </si>
   <si>
@@ -880,6 +940,9 @@
     <t xml:space="preserve">P224</t>
   </si>
   <si>
+    <t xml:space="preserve">C25_ane_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P225</t>
   </si>
   <si>
@@ -898,6 +961,9 @@
     <t xml:space="preserve">P230</t>
   </si>
   <si>
+    <t xml:space="preserve">C26_ene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P231</t>
   </si>
   <si>
@@ -907,6 +973,9 @@
     <t xml:space="preserve">P233</t>
   </si>
   <si>
+    <t xml:space="preserve">C26_ane_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P234</t>
   </si>
   <si>
@@ -928,6 +997,9 @@
     <t xml:space="preserve">P240</t>
   </si>
   <si>
+    <t xml:space="preserve">C27_ene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P241</t>
   </si>
   <si>
@@ -937,12 +1009,18 @@
     <t xml:space="preserve">P243</t>
   </si>
   <si>
+    <t xml:space="preserve">C27_ane_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P244</t>
   </si>
   <si>
     <t xml:space="preserve">P245</t>
   </si>
   <si>
+    <t xml:space="preserve">C27_Me_11-;13-</t>
+  </si>
+  <si>
     <t xml:space="preserve">P246</t>
   </si>
   <si>
@@ -967,6 +1045,9 @@
     <t xml:space="preserve">P253</t>
   </si>
   <si>
+    <t xml:space="preserve">C28_ane_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P254</t>
   </si>
   <si>
@@ -991,6 +1072,9 @@
     <t xml:space="preserve">P261</t>
   </si>
   <si>
+    <t xml:space="preserve">C29_ene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P262</t>
   </si>
   <si>
@@ -1000,12 +1084,18 @@
     <t xml:space="preserve">P264</t>
   </si>
   <si>
+    <t xml:space="preserve">C29_ane_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P265</t>
   </si>
   <si>
     <t xml:space="preserve">P266</t>
   </si>
   <si>
+    <t xml:space="preserve">C29_Me_13-</t>
+  </si>
+  <si>
     <t xml:space="preserve">P267</t>
   </si>
   <si>
@@ -1021,12 +1111,18 @@
     <t xml:space="preserve">P271</t>
   </si>
   <si>
+    <t xml:space="preserve">C30_ene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P272</t>
   </si>
   <si>
     <t xml:space="preserve">P273</t>
   </si>
   <si>
+    <t xml:space="preserve">C30_ane_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P274</t>
   </si>
   <si>
@@ -1045,9 +1141,15 @@
     <t xml:space="preserve">P279</t>
   </si>
   <si>
+    <t xml:space="preserve">C31_diene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P280</t>
   </si>
   <si>
+    <t xml:space="preserve">C31_ene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P281</t>
   </si>
   <si>
@@ -1057,10 +1159,16 @@
     <t xml:space="preserve">P283</t>
   </si>
   <si>
+    <t xml:space="preserve">C31_ane_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P284</t>
   </si>
   <si>
     <t xml:space="preserve">P285</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C31_Me_13-;15-</t>
   </si>
   <si>
     <t xml:space="preserve">P286</t>
@@ -1286,7 +1394,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1297,6 +1405,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF7B59"/>
         <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -1334,7 +1448,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1344,6 +1458,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1427,14 +1545,14 @@
   <dimension ref="A1:AQ350"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A259" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D187" activeCellId="0" sqref="D187"/>
+      <selection pane="bottomLeft" activeCell="AN286" activeCellId="0" sqref="AN286"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12167,7 +12285,9 @@
       <c r="A196" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="B196" s="1"/>
+      <c r="B196" s="1" t="s">
+        <v>249</v>
+      </c>
       <c r="C196" s="1" t="n">
         <v>32.4177027027027</v>
       </c>
@@ -12189,7 +12309,7 @@
       <c r="I196" s="1" t="n">
         <v>32.427</v>
       </c>
-      <c r="K196" s="1" t="n">
+      <c r="K196" s="2" t="n">
         <v>32.434</v>
       </c>
       <c r="L196" s="1" t="n">
@@ -12285,9 +12405,11 @@
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="B197" s="1"/>
+        <v>250</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="C197" s="1" t="n">
         <v>32.516275</v>
       </c>
@@ -12414,9 +12536,11 @@
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="B198" s="1"/>
+        <v>252</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="C198" s="1" t="n">
         <v>32.6291</v>
       </c>
@@ -12543,9 +12667,9 @@
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="B199" s="1"/>
+        <v>253</v>
+      </c>
+      <c r="B199" s="3"/>
       <c r="C199" s="1" t="n">
         <v>32.763425</v>
       </c>
@@ -12672,7 +12796,7 @@
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B200" s="1"/>
       <c r="C200" s="1" t="n">
@@ -12684,9 +12808,11 @@
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="B201" s="1"/>
+        <v>255</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>256</v>
+      </c>
       <c r="C201" s="1" t="n">
         <v>33.036475</v>
       </c>
@@ -12813,7 +12939,7 @@
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="1" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B202" s="1"/>
       <c r="C202" s="1" t="n">
@@ -12879,7 +13005,7 @@
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B203" s="1"/>
       <c r="C203" s="1" t="n">
@@ -12939,7 +13065,7 @@
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="1" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B204" s="1"/>
       <c r="C204" s="1" t="n">
@@ -13068,7 +13194,7 @@
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B205" s="1"/>
       <c r="C205" s="1" t="n">
@@ -13197,7 +13323,7 @@
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="1" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B206" s="1"/>
       <c r="C206" s="1" t="n">
@@ -13239,7 +13365,7 @@
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="1" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B207" s="1"/>
       <c r="C207" s="1" t="n">
@@ -13254,7 +13380,7 @@
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="1" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B208" s="1"/>
       <c r="C208" s="1" t="n">
@@ -13320,9 +13446,11 @@
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="B209" s="1"/>
+        <v>264</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>265</v>
+      </c>
       <c r="C209" s="1" t="n">
         <v>34.1364</v>
       </c>
@@ -13449,7 +13577,7 @@
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="1" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="B210" s="1"/>
       <c r="C210" s="1" t="n">
@@ -13566,7 +13694,7 @@
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="1" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="B211" s="1"/>
       <c r="C211" s="1" t="n">
@@ -13659,7 +13787,7 @@
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="1" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="B212" s="1"/>
       <c r="C212" s="1" t="n">
@@ -13677,9 +13805,11 @@
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="B213" s="1"/>
+        <v>269</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>270</v>
+      </c>
       <c r="C213" s="1" t="n">
         <v>34.566175</v>
       </c>
@@ -13806,7 +13936,7 @@
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="1" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="B214" s="1"/>
       <c r="C214" s="1" t="n">
@@ -13845,7 +13975,7 @@
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="1" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="B215" s="1"/>
       <c r="C215" s="1" t="n">
@@ -13881,7 +14011,7 @@
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="1" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="B216" s="1"/>
       <c r="C216" s="1" t="n">
@@ -14007,7 +14137,7 @@
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="1" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="B217" s="1"/>
       <c r="C217" s="1" t="n">
@@ -14061,7 +14191,7 @@
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="1" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="B218" s="1"/>
       <c r="C218" s="1" t="n">
@@ -14154,7 +14284,7 @@
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="1" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="B219" s="1"/>
       <c r="C219" s="1" t="n">
@@ -14211,7 +14341,7 @@
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="1" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="B220" s="1"/>
       <c r="C220" s="1" t="n">
@@ -14274,7 +14404,7 @@
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="1" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="B221" s="1"/>
       <c r="C221" s="1" t="n">
@@ -14286,9 +14416,11 @@
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="B222" s="1"/>
+        <v>279</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>280</v>
+      </c>
       <c r="C222" s="1" t="n">
         <v>35.72025</v>
       </c>
@@ -14415,9 +14547,11 @@
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="B223" s="1"/>
+        <v>281</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>280</v>
+      </c>
       <c r="C223" s="1" t="n">
         <v>35.83845</v>
       </c>
@@ -14544,7 +14678,7 @@
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="1" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="B224" s="1"/>
       <c r="C224" s="1" t="n">
@@ -14574,9 +14708,11 @@
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="B225" s="1"/>
+        <v>283</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>284</v>
+      </c>
       <c r="C225" s="1" t="n">
         <v>36.19115</v>
       </c>
@@ -14703,7 +14839,7 @@
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="1" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="B226" s="1"/>
       <c r="C226" s="1" t="n">
@@ -14790,7 +14926,7 @@
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="1" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="B227" s="1"/>
       <c r="C227" s="1" t="n">
@@ -14919,7 +15055,7 @@
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="1" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="B228" s="1"/>
       <c r="C228" s="1" t="n">
@@ -15045,7 +15181,7 @@
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="B229" s="1"/>
       <c r="C229" s="1" t="n">
@@ -15057,7 +15193,7 @@
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="1" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="B230" s="1"/>
       <c r="C230" s="1" t="n">
@@ -15132,9 +15268,11 @@
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="B231" s="1"/>
+        <v>290</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>291</v>
+      </c>
       <c r="C231" s="1" t="n">
         <v>37.2255769230769</v>
       </c>
@@ -15219,9 +15357,9 @@
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="B232" s="1"/>
+        <v>292</v>
+      </c>
+      <c r="B232" s="3"/>
       <c r="C232" s="1" t="n">
         <v>37.3364</v>
       </c>
@@ -15348,7 +15486,7 @@
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="1" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="B233" s="1"/>
       <c r="C233" s="1" t="n">
@@ -15363,9 +15501,11 @@
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="B234" s="1"/>
+        <v>294</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>295</v>
+      </c>
       <c r="C234" s="1" t="n">
         <v>37.61365</v>
       </c>
@@ -15492,7 +15632,7 @@
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="1" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="B235" s="1"/>
       <c r="C235" s="1" t="n">
@@ -15516,7 +15656,7 @@
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="1" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
       <c r="B236" s="1"/>
       <c r="C236" s="1" t="n">
@@ -15528,7 +15668,7 @@
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="1" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="B237" s="1"/>
       <c r="C237" s="1" t="n">
@@ -15651,7 +15791,7 @@
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="1" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="B238" s="1"/>
       <c r="C238" s="1" t="n">
@@ -15753,7 +15893,7 @@
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="1" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="B239" s="1"/>
       <c r="C239" s="1" t="n">
@@ -15849,7 +15989,7 @@
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="1" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
       <c r="B240" s="1"/>
       <c r="C240" s="1" t="n">
@@ -15963,9 +16103,11 @@
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="B241" s="1"/>
+        <v>302</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>303</v>
+      </c>
       <c r="C241" s="1" t="n">
         <v>38.69745</v>
       </c>
@@ -16092,9 +16234,11 @@
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="B242" s="1"/>
+        <v>304</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>303</v>
+      </c>
       <c r="C242" s="1" t="n">
         <v>38.8101</v>
       </c>
@@ -16221,7 +16365,7 @@
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="1" t="s">
-        <v>295</v>
+        <v>305</v>
       </c>
       <c r="B243" s="1"/>
       <c r="C243" s="1" t="n">
@@ -16251,9 +16395,11 @@
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="B244" s="1"/>
+        <v>306</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>307</v>
+      </c>
       <c r="C244" s="1" t="n">
         <v>39.118975</v>
       </c>
@@ -16380,7 +16526,7 @@
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="1" t="s">
-        <v>297</v>
+        <v>308</v>
       </c>
       <c r="B245" s="1"/>
       <c r="C245" s="1" t="n">
@@ -16419,9 +16565,11 @@
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="B246" s="1"/>
+        <v>309</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="C246" s="1" t="n">
         <v>39.514375</v>
       </c>
@@ -16548,7 +16696,7 @@
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="1" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
       <c r="B247" s="1"/>
       <c r="C247" s="1" t="n">
@@ -16560,7 +16708,7 @@
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="1" t="s">
-        <v>300</v>
+        <v>312</v>
       </c>
       <c r="B248" s="1"/>
       <c r="C248" s="1" t="n">
@@ -16641,7 +16789,7 @@
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="1" t="s">
-        <v>301</v>
+        <v>313</v>
       </c>
       <c r="B249" s="1"/>
       <c r="C249" s="1" t="n">
@@ -16662,7 +16810,7 @@
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="1" t="s">
-        <v>302</v>
+        <v>314</v>
       </c>
       <c r="B250" s="1"/>
       <c r="C250" s="1" t="n">
@@ -16740,7 +16888,7 @@
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="1" t="s">
-        <v>303</v>
+        <v>315</v>
       </c>
       <c r="B251" s="1"/>
       <c r="C251" s="1" t="n">
@@ -16770,7 +16918,7 @@
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="1" t="s">
-        <v>304</v>
+        <v>316</v>
       </c>
       <c r="B252" s="1"/>
       <c r="C252" s="1" t="n">
@@ -16899,7 +17047,7 @@
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="1" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
       <c r="B253" s="1"/>
       <c r="C253" s="1" t="n">
@@ -16923,9 +17071,11 @@
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="B254" s="1"/>
+        <v>318</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>319</v>
+      </c>
       <c r="C254" s="1" t="n">
         <v>40.441125</v>
       </c>
@@ -17052,7 +17202,7 @@
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="1" t="s">
-        <v>307</v>
+        <v>320</v>
       </c>
       <c r="B255" s="1"/>
       <c r="C255" s="1" t="n">
@@ -17064,7 +17214,7 @@
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="1" t="s">
-        <v>308</v>
+        <v>321</v>
       </c>
       <c r="B256" s="1"/>
       <c r="C256" s="1" t="n">
@@ -17091,7 +17241,7 @@
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="1" t="s">
-        <v>309</v>
+        <v>322</v>
       </c>
       <c r="B257" s="1"/>
       <c r="C257" s="1" t="n">
@@ -17220,7 +17370,7 @@
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="1" t="s">
-        <v>310</v>
+        <v>323</v>
       </c>
       <c r="B258" s="1"/>
       <c r="C258" s="1" t="n">
@@ -17238,7 +17388,7 @@
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="1" t="s">
-        <v>311</v>
+        <v>324</v>
       </c>
       <c r="B259" s="1"/>
       <c r="C259" s="1" t="n">
@@ -17364,7 +17514,7 @@
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="1" t="s">
-        <v>312</v>
+        <v>325</v>
       </c>
       <c r="B260" s="1"/>
       <c r="C260" s="1" t="n">
@@ -17448,7 +17598,7 @@
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="1" t="s">
-        <v>313</v>
+        <v>326</v>
       </c>
       <c r="B261" s="1"/>
       <c r="C261" s="1" t="n">
@@ -17535,9 +17685,11 @@
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="B262" s="1"/>
+        <v>327</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>328</v>
+      </c>
       <c r="C262" s="1" t="n">
         <v>41.4770434782609</v>
       </c>
@@ -17613,9 +17765,11 @@
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="B263" s="1"/>
+        <v>329</v>
+      </c>
+      <c r="B263" s="1" t="s">
+        <v>328</v>
+      </c>
       <c r="C263" s="1" t="n">
         <v>41.5287777777778</v>
       </c>
@@ -17730,7 +17884,7 @@
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="1" t="s">
-        <v>316</v>
+        <v>330</v>
       </c>
       <c r="B264" s="1"/>
       <c r="C264" s="1" t="n">
@@ -17742,9 +17896,11 @@
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="B265" s="1"/>
+        <v>331</v>
+      </c>
+      <c r="B265" s="1" t="s">
+        <v>332</v>
+      </c>
       <c r="C265" s="1" t="n">
         <v>41.82435</v>
       </c>
@@ -17871,7 +18027,7 @@
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="1" t="s">
-        <v>318</v>
+        <v>333</v>
       </c>
       <c r="B266" s="1"/>
       <c r="C266" s="1" t="n">
@@ -17937,9 +18093,11 @@
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="B267" s="1"/>
+        <v>334</v>
+      </c>
+      <c r="B267" s="3" t="s">
+        <v>335</v>
+      </c>
       <c r="C267" s="1" t="n">
         <v>42.195725</v>
       </c>
@@ -18066,7 +18224,7 @@
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="1" t="s">
-        <v>320</v>
+        <v>336</v>
       </c>
       <c r="B268" s="1"/>
       <c r="C268" s="1" t="n">
@@ -18087,7 +18245,7 @@
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="1" t="s">
-        <v>321</v>
+        <v>337</v>
       </c>
       <c r="B269" s="1"/>
       <c r="C269" s="1" t="n">
@@ -18177,7 +18335,7 @@
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="1" t="s">
-        <v>322</v>
+        <v>338</v>
       </c>
       <c r="B270" s="1"/>
       <c r="C270" s="1" t="n">
@@ -18294,7 +18452,7 @@
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="1" t="s">
-        <v>323</v>
+        <v>339</v>
       </c>
       <c r="B271" s="1"/>
       <c r="C271" s="1" t="n">
@@ -18333,28 +18491,30 @@
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="B272" s="1"/>
+        <v>340</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>341</v>
+      </c>
       <c r="C272" s="1" t="n">
         <v>42.8910555555556</v>
       </c>
-      <c r="D272" s="1" t="n">
+      <c r="D272" s="2" t="n">
         <v>42.922</v>
       </c>
-      <c r="E272" s="1" t="n">
+      <c r="E272" s="2" t="n">
         <v>42.901</v>
       </c>
-      <c r="F272" s="1" t="n">
+      <c r="F272" s="2" t="n">
         <v>42.908</v>
       </c>
-      <c r="G272" s="1" t="n">
+      <c r="G272" s="2" t="n">
         <v>42.894</v>
       </c>
-      <c r="H272" s="1" t="n">
+      <c r="H272" s="2" t="n">
         <v>42.901</v>
       </c>
-      <c r="I272" s="1" t="n">
+      <c r="I272" s="2" t="n">
         <v>42.902</v>
       </c>
       <c r="J272" s="1" t="n">
@@ -18369,16 +18529,16 @@
       <c r="M272" s="1" t="n">
         <v>42.895</v>
       </c>
-      <c r="N272" s="1" t="n">
+      <c r="N272" s="2" t="n">
         <v>42.895</v>
       </c>
       <c r="O272" s="1" t="n">
         <v>42.888</v>
       </c>
-      <c r="P272" s="1" t="n">
+      <c r="P272" s="2" t="n">
         <v>42.908</v>
       </c>
-      <c r="Q272" s="1" t="n">
+      <c r="Q272" s="2" t="n">
         <v>42.901</v>
       </c>
       <c r="R272" s="1" t="n">
@@ -18396,13 +18556,13 @@
       <c r="V272" s="1" t="n">
         <v>42.881</v>
       </c>
-      <c r="W272" s="1" t="n">
+      <c r="W272" s="2" t="n">
         <v>42.901</v>
       </c>
       <c r="X272" s="1" t="n">
         <v>42.901</v>
       </c>
-      <c r="Y272" s="1" t="n">
+      <c r="Y272" s="2" t="n">
         <v>42.895</v>
       </c>
       <c r="Z272" s="1" t="n">
@@ -18450,7 +18610,7 @@
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="1" t="s">
-        <v>325</v>
+        <v>342</v>
       </c>
       <c r="B273" s="1"/>
       <c r="C273" s="1" t="n">
@@ -18525,9 +18685,11 @@
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="B274" s="1"/>
+        <v>343</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>344</v>
+      </c>
       <c r="C274" s="1" t="n">
         <v>43.0808484848485</v>
       </c>
@@ -18633,7 +18795,7 @@
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="1" t="s">
-        <v>327</v>
+        <v>345</v>
       </c>
       <c r="B275" s="1"/>
       <c r="C275" s="1" t="n">
@@ -18645,7 +18807,7 @@
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="1" t="s">
-        <v>328</v>
+        <v>346</v>
       </c>
       <c r="B276" s="1"/>
       <c r="C276" s="1" t="n">
@@ -18717,7 +18879,7 @@
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="1" t="s">
-        <v>329</v>
+        <v>347</v>
       </c>
       <c r="B277" s="1"/>
       <c r="C277" s="1" t="n">
@@ -18798,7 +18960,7 @@
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="1" t="s">
-        <v>330</v>
+        <v>348</v>
       </c>
       <c r="B278" s="1"/>
       <c r="C278" s="1" t="n">
@@ -18810,7 +18972,7 @@
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="1" t="s">
-        <v>331</v>
+        <v>349</v>
       </c>
       <c r="B279" s="1"/>
       <c r="C279" s="1" t="n">
@@ -18879,9 +19041,11 @@
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="B280" s="1"/>
+        <v>350</v>
+      </c>
+      <c r="B280" s="3" t="s">
+        <v>351</v>
+      </c>
       <c r="C280" s="1" t="n">
         <v>43.842675</v>
       </c>
@@ -19008,9 +19172,11 @@
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="B281" s="1"/>
+        <v>352</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>353</v>
+      </c>
       <c r="C281" s="1" t="n">
         <v>44.0389</v>
       </c>
@@ -19137,9 +19303,11 @@
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="B282" s="1"/>
+        <v>354</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>353</v>
+      </c>
       <c r="C282" s="1" t="n">
         <v>44.13325</v>
       </c>
@@ -19266,7 +19434,7 @@
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="1" t="s">
-        <v>335</v>
+        <v>355</v>
       </c>
       <c r="B283" s="1"/>
       <c r="C283" s="1" t="n">
@@ -19296,9 +19464,11 @@
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="B284" s="1"/>
+        <v>356</v>
+      </c>
+      <c r="B284" s="1" t="s">
+        <v>357</v>
+      </c>
       <c r="C284" s="1" t="n">
         <v>44.356925</v>
       </c>
@@ -19425,7 +19595,7 @@
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="1" t="s">
-        <v>337</v>
+        <v>358</v>
       </c>
       <c r="B285" s="1"/>
       <c r="C285" s="1" t="n">
@@ -19440,9 +19610,11 @@
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="B286" s="1"/>
+        <v>359</v>
+      </c>
+      <c r="B286" s="1" t="s">
+        <v>360</v>
+      </c>
       <c r="C286" s="1" t="n">
         <v>44.6850263157895</v>
       </c>
@@ -19458,7 +19630,7 @@
       <c r="I286" s="1" t="n">
         <v>44.715</v>
       </c>
-      <c r="J286" s="1" t="n">
+      <c r="J286" s="3" t="n">
         <v>44.666</v>
       </c>
       <c r="K286" s="1" t="n">
@@ -19473,7 +19645,7 @@
       <c r="N286" s="1" t="n">
         <v>44.701</v>
       </c>
-      <c r="O286" s="1" t="n">
+      <c r="O286" s="3" t="n">
         <v>44.653</v>
       </c>
       <c r="P286" s="1" t="n">
@@ -19482,88 +19654,88 @@
       <c r="Q286" s="1" t="n">
         <v>44.722</v>
       </c>
-      <c r="R286" s="1" t="n">
+      <c r="R286" s="3" t="n">
         <v>44.667</v>
       </c>
       <c r="S286" s="1" t="n">
         <v>44.708</v>
       </c>
-      <c r="T286" s="1" t="n">
+      <c r="T286" s="3" t="n">
         <v>44.667</v>
       </c>
-      <c r="U286" s="1" t="n">
+      <c r="U286" s="3" t="n">
         <v>44.66</v>
       </c>
-      <c r="V286" s="1" t="n">
+      <c r="V286" s="3" t="n">
         <v>44.66</v>
       </c>
       <c r="W286" s="1" t="n">
         <v>44.722</v>
       </c>
-      <c r="X286" s="1" t="n">
+      <c r="X286" s="3" t="n">
         <v>44.66</v>
       </c>
       <c r="Y286" s="1" t="n">
         <v>44.708</v>
       </c>
-      <c r="Z286" s="1" t="n">
+      <c r="Z286" s="3" t="n">
         <v>44.646</v>
       </c>
-      <c r="AA286" s="1" t="n">
+      <c r="AA286" s="3" t="n">
         <v>44.701</v>
       </c>
-      <c r="AB286" s="1" t="n">
+      <c r="AB286" s="3" t="n">
         <v>44.66</v>
       </c>
-      <c r="AC286" s="1" t="n">
+      <c r="AC286" s="3" t="n">
         <v>44.659</v>
       </c>
-      <c r="AD286" s="1" t="n">
+      <c r="AD286" s="3" t="n">
         <v>44.674</v>
       </c>
-      <c r="AE286" s="1" t="n">
+      <c r="AE286" s="3" t="n">
         <v>44.715</v>
       </c>
-      <c r="AF286" s="1" t="n">
+      <c r="AF286" s="3" t="n">
         <v>44.667</v>
       </c>
       <c r="AG286" s="1" t="n">
         <v>44.715</v>
       </c>
-      <c r="AH286" s="1" t="n">
+      <c r="AH286" s="3" t="n">
         <v>44.667</v>
       </c>
-      <c r="AI286" s="1" t="n">
+      <c r="AI286" s="3" t="n">
         <v>44.66</v>
       </c>
-      <c r="AJ286" s="1" t="n">
+      <c r="AJ286" s="3" t="n">
         <v>44.715</v>
       </c>
-      <c r="AK286" s="1" t="n">
+      <c r="AK286" s="3" t="n">
         <v>44.653</v>
       </c>
       <c r="AL286" s="1" t="n">
         <v>44.715</v>
       </c>
-      <c r="AM286" s="1" t="n">
+      <c r="AM286" s="3" t="n">
         <v>44.66</v>
       </c>
-      <c r="AN286" s="1" t="n">
+      <c r="AN286" s="3" t="n">
         <v>44.653</v>
       </c>
       <c r="AO286" s="1" t="n">
         <v>44.708</v>
       </c>
-      <c r="AP286" s="1" t="n">
+      <c r="AP286" s="3" t="n">
         <v>44.646</v>
       </c>
-      <c r="AQ286" s="1" t="n">
+      <c r="AQ286" s="3" t="n">
         <v>44.646</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="1" t="s">
-        <v>339</v>
+        <v>361</v>
       </c>
       <c r="B287" s="1"/>
       <c r="C287" s="1" t="n">
@@ -19575,7 +19747,7 @@
       <c r="E287" s="1" t="n">
         <v>44.798</v>
       </c>
-      <c r="F287" s="1" t="n">
+      <c r="F287" s="3" t="n">
         <v>44.791</v>
       </c>
       <c r="G287" s="1" t="n">
@@ -19614,7 +19786,7 @@
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="1" t="s">
-        <v>340</v>
+        <v>362</v>
       </c>
       <c r="B288" s="1"/>
       <c r="C288" s="1" t="n">
@@ -19674,7 +19846,7 @@
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="1" t="s">
-        <v>341</v>
+        <v>363</v>
       </c>
       <c r="B289" s="1"/>
       <c r="C289" s="1" t="n">
@@ -19740,7 +19912,7 @@
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="1" t="s">
-        <v>342</v>
+        <v>364</v>
       </c>
       <c r="B290" s="1"/>
       <c r="C290" s="1" t="n">
@@ -19839,7 +20011,7 @@
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="1" t="s">
-        <v>343</v>
+        <v>365</v>
       </c>
       <c r="B291" s="1"/>
       <c r="C291" s="1" t="n">
@@ -19851,7 +20023,7 @@
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="1" t="s">
-        <v>344</v>
+        <v>366</v>
       </c>
       <c r="B292" s="1"/>
       <c r="C292" s="1" t="n">
@@ -19902,7 +20074,7 @@
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="1" t="s">
-        <v>345</v>
+        <v>367</v>
       </c>
       <c r="B293" s="1"/>
       <c r="C293" s="1" t="n">
@@ -20028,7 +20200,7 @@
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="1" t="s">
-        <v>346</v>
+        <v>368</v>
       </c>
       <c r="B294" s="1"/>
       <c r="C294" s="1" t="n">
@@ -20127,7 +20299,7 @@
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="1" t="s">
-        <v>347</v>
+        <v>369</v>
       </c>
       <c r="B295" s="1"/>
       <c r="C295" s="1" t="n">
@@ -20175,7 +20347,7 @@
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="1" t="s">
-        <v>348</v>
+        <v>370</v>
       </c>
       <c r="B296" s="1"/>
       <c r="C296" s="1" t="n">
@@ -20205,7 +20377,7 @@
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="1" t="s">
-        <v>349</v>
+        <v>371</v>
       </c>
       <c r="B297" s="1"/>
       <c r="C297" s="1" t="n">
@@ -20334,7 +20506,7 @@
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="1" t="s">
-        <v>350</v>
+        <v>372</v>
       </c>
       <c r="B298" s="1"/>
       <c r="C298" s="1" t="n">
@@ -20463,7 +20635,7 @@
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="1" t="s">
-        <v>351</v>
+        <v>373</v>
       </c>
       <c r="B299" s="1"/>
       <c r="C299" s="1" t="n">
@@ -20520,7 +20692,7 @@
     </row>
     <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="1" t="s">
-        <v>352</v>
+        <v>374</v>
       </c>
       <c r="B300" s="1"/>
       <c r="C300" s="1" t="n">
@@ -20631,7 +20803,7 @@
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="1" t="s">
-        <v>353</v>
+        <v>375</v>
       </c>
       <c r="B301" s="1"/>
       <c r="C301" s="1" t="n">
@@ -20646,7 +20818,7 @@
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="1" t="s">
-        <v>354</v>
+        <v>376</v>
       </c>
       <c r="B302" s="1"/>
       <c r="C302" s="1" t="n">
@@ -20775,7 +20947,7 @@
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="1" t="s">
-        <v>355</v>
+        <v>377</v>
       </c>
       <c r="B303" s="1"/>
       <c r="C303" s="1" t="n">
@@ -20808,7 +20980,7 @@
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="1" t="s">
-        <v>356</v>
+        <v>378</v>
       </c>
       <c r="B304" s="1"/>
       <c r="C304" s="1" t="n">
@@ -20937,7 +21109,7 @@
     </row>
     <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="1" t="s">
-        <v>357</v>
+        <v>379</v>
       </c>
       <c r="B305" s="1"/>
       <c r="C305" s="1" t="n">
@@ -20970,7 +21142,7 @@
     </row>
     <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="1" t="s">
-        <v>358</v>
+        <v>380</v>
       </c>
       <c r="B306" s="1"/>
       <c r="C306" s="1" t="n">
@@ -21045,7 +21217,7 @@
     </row>
     <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="1" t="s">
-        <v>359</v>
+        <v>381</v>
       </c>
       <c r="B307" s="1"/>
       <c r="C307" s="1" t="n">
@@ -21141,7 +21313,7 @@
     </row>
     <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="1" t="s">
-        <v>360</v>
+        <v>382</v>
       </c>
       <c r="B308" s="1"/>
       <c r="C308" s="1" t="n">
@@ -21213,7 +21385,7 @@
     </row>
     <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="1" t="s">
-        <v>361</v>
+        <v>383</v>
       </c>
       <c r="B309" s="1"/>
       <c r="C309" s="1" t="n">
@@ -21321,7 +21493,7 @@
     </row>
     <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="1" t="s">
-        <v>362</v>
+        <v>384</v>
       </c>
       <c r="B310" s="1"/>
       <c r="C310" s="1" t="n">
@@ -21357,7 +21529,7 @@
     </row>
     <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="1" t="s">
-        <v>363</v>
+        <v>385</v>
       </c>
       <c r="B311" s="1"/>
       <c r="C311" s="1" t="n">
@@ -21405,7 +21577,7 @@
     </row>
     <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="1" t="s">
-        <v>364</v>
+        <v>386</v>
       </c>
       <c r="B312" s="1"/>
       <c r="C312" s="1" t="n">
@@ -21420,7 +21592,7 @@
     </row>
     <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="1" t="s">
-        <v>365</v>
+        <v>387</v>
       </c>
       <c r="B313" s="1"/>
       <c r="C313" s="1" t="n">
@@ -21435,7 +21607,7 @@
     </row>
     <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="1" t="s">
-        <v>366</v>
+        <v>388</v>
       </c>
       <c r="B314" s="1"/>
       <c r="C314" s="1" t="n">
@@ -21561,7 +21733,7 @@
     </row>
     <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="1" t="s">
-        <v>367</v>
+        <v>389</v>
       </c>
       <c r="B315" s="1"/>
       <c r="C315" s="1" t="n">
@@ -21624,7 +21796,7 @@
     </row>
     <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="1" t="s">
-        <v>368</v>
+        <v>390</v>
       </c>
       <c r="B316" s="1"/>
       <c r="C316" s="1" t="n">
@@ -21711,7 +21883,7 @@
     </row>
     <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="1" t="s">
-        <v>369</v>
+        <v>391</v>
       </c>
       <c r="B317" s="1"/>
       <c r="C317" s="1" t="n">
@@ -21774,7 +21946,7 @@
     </row>
     <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="1" t="s">
-        <v>370</v>
+        <v>392</v>
       </c>
       <c r="B318" s="1"/>
       <c r="C318" s="1" t="n">
@@ -21897,7 +22069,7 @@
     </row>
     <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="1" t="s">
-        <v>371</v>
+        <v>393</v>
       </c>
       <c r="B319" s="1"/>
       <c r="C319" s="1" t="n">
@@ -21909,7 +22081,7 @@
     </row>
     <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="1" t="s">
-        <v>372</v>
+        <v>394</v>
       </c>
       <c r="B320" s="1"/>
       <c r="C320" s="1" t="n">
@@ -21921,7 +22093,7 @@
     </row>
     <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="1" t="s">
-        <v>373</v>
+        <v>395</v>
       </c>
       <c r="B321" s="1"/>
       <c r="C321" s="1" t="n">
@@ -21963,7 +22135,7 @@
     </row>
     <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="1" t="s">
-        <v>374</v>
+        <v>396</v>
       </c>
       <c r="B322" s="1"/>
       <c r="C322" s="1" t="n">
@@ -21984,7 +22156,7 @@
     </row>
     <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="1" t="s">
-        <v>375</v>
+        <v>397</v>
       </c>
       <c r="B323" s="1"/>
       <c r="C323" s="1" t="n">
@@ -22014,7 +22186,7 @@
     </row>
     <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="1" t="s">
-        <v>376</v>
+        <v>398</v>
       </c>
       <c r="B324" s="1"/>
       <c r="C324" s="1" t="n">
@@ -22104,7 +22276,7 @@
     </row>
     <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="1" t="s">
-        <v>377</v>
+        <v>399</v>
       </c>
       <c r="B325" s="1"/>
       <c r="C325" s="1" t="n">
@@ -22158,7 +22330,7 @@
     </row>
     <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="1" t="s">
-        <v>378</v>
+        <v>400</v>
       </c>
       <c r="B326" s="1"/>
       <c r="C326" s="1" t="n">
@@ -22215,7 +22387,7 @@
     </row>
     <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="1" t="s">
-        <v>379</v>
+        <v>401</v>
       </c>
       <c r="B327" s="1"/>
       <c r="C327" s="1" t="n">
@@ -22230,7 +22402,7 @@
     </row>
     <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="1" t="s">
-        <v>380</v>
+        <v>402</v>
       </c>
       <c r="B328" s="1"/>
       <c r="C328" s="1" t="n">
@@ -22335,7 +22507,7 @@
     </row>
     <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="1" t="s">
-        <v>381</v>
+        <v>403</v>
       </c>
       <c r="B329" s="1"/>
       <c r="C329" s="1" t="n">
@@ -22437,7 +22609,7 @@
     </row>
     <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="1" t="s">
-        <v>382</v>
+        <v>404</v>
       </c>
       <c r="B330" s="1"/>
       <c r="C330" s="1" t="n">
@@ -22449,7 +22621,7 @@
     </row>
     <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="1" t="s">
-        <v>383</v>
+        <v>405</v>
       </c>
       <c r="B331" s="1"/>
       <c r="C331" s="1" t="n">
@@ -22461,7 +22633,7 @@
     </row>
     <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="1" t="s">
-        <v>384</v>
+        <v>406</v>
       </c>
       <c r="B332" s="1"/>
       <c r="C332" s="1" t="n">
@@ -22536,7 +22708,7 @@
     </row>
     <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="1" t="s">
-        <v>385</v>
+        <v>407</v>
       </c>
       <c r="B333" s="1"/>
       <c r="C333" s="1" t="n">
@@ -22548,7 +22720,7 @@
     </row>
     <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="1" t="s">
-        <v>386</v>
+        <v>408</v>
       </c>
       <c r="B334" s="1"/>
       <c r="C334" s="1" t="n">
@@ -22563,7 +22735,7 @@
     </row>
     <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="1" t="s">
-        <v>387</v>
+        <v>409</v>
       </c>
       <c r="B335" s="1"/>
       <c r="C335" s="1" t="n">
@@ -22581,7 +22753,7 @@
     </row>
     <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="1" t="s">
-        <v>388</v>
+        <v>410</v>
       </c>
       <c r="B336" s="1"/>
       <c r="C336" s="1" t="n">
@@ -22710,7 +22882,7 @@
     </row>
     <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="1" t="s">
-        <v>389</v>
+        <v>411</v>
       </c>
       <c r="B337" s="1"/>
       <c r="C337" s="1" t="n">
@@ -22734,7 +22906,7 @@
     </row>
     <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="1" t="s">
-        <v>390</v>
+        <v>412</v>
       </c>
       <c r="B338" s="1"/>
       <c r="C338" s="1" t="n">
@@ -22809,7 +22981,7 @@
     </row>
     <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="1" t="s">
-        <v>391</v>
+        <v>413</v>
       </c>
       <c r="B339" s="1"/>
       <c r="C339" s="1" t="n">
@@ -22854,7 +23026,7 @@
     </row>
     <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="1" t="s">
-        <v>392</v>
+        <v>414</v>
       </c>
       <c r="B340" s="1"/>
       <c r="C340" s="1" t="n">
@@ -22866,7 +23038,7 @@
     </row>
     <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="1" t="s">
-        <v>393</v>
+        <v>415</v>
       </c>
       <c r="B341" s="1"/>
       <c r="C341" s="1" t="n">
@@ -22917,7 +23089,7 @@
     </row>
     <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="1" t="s">
-        <v>394</v>
+        <v>416</v>
       </c>
       <c r="B342" s="1"/>
       <c r="C342" s="1" t="n">
@@ -22932,7 +23104,7 @@
     </row>
     <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="1" t="s">
-        <v>395</v>
+        <v>417</v>
       </c>
       <c r="B343" s="1"/>
       <c r="C343" s="1" t="n">
@@ -22959,7 +23131,7 @@
     </row>
     <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="1" t="s">
-        <v>396</v>
+        <v>418</v>
       </c>
       <c r="B344" s="1"/>
       <c r="C344" s="1" t="n">
@@ -22974,7 +23146,7 @@
     </row>
     <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="1" t="s">
-        <v>397</v>
+        <v>419</v>
       </c>
       <c r="B345" s="1"/>
       <c r="C345" s="1" t="n">
@@ -23046,7 +23218,7 @@
     </row>
     <row r="346" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="1" t="s">
-        <v>398</v>
+        <v>420</v>
       </c>
       <c r="B346" s="1"/>
       <c r="C346" s="1" t="n">
@@ -23175,7 +23347,7 @@
     </row>
     <row r="347" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="1" t="s">
-        <v>399</v>
+        <v>421</v>
       </c>
       <c r="B347" s="1"/>
       <c r="C347" s="1" t="n">
@@ -23241,7 +23413,7 @@
     </row>
     <row r="348" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="1" t="s">
-        <v>400</v>
+        <v>422</v>
       </c>
       <c r="B348" s="1"/>
       <c r="C348" s="1" t="n">
@@ -23256,7 +23428,7 @@
     </row>
     <row r="349" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="1" t="s">
-        <v>401</v>
+        <v>423</v>
       </c>
       <c r="B349" s="1"/>
       <c r="C349" s="1" t="n">
@@ -23268,7 +23440,7 @@
     </row>
     <row r="350" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="1" t="s">
-        <v>402</v>
+        <v>424</v>
       </c>
       <c r="B350" s="1"/>
       <c r="C350" s="1" t="n">

</xml_diff>

<commit_message>
Continuation of CHC identification for Br Ib.
</commit_message>
<xml_diff>
--- a/data/raw/NM-recognition/tmp/Br_Ib_RT_ID_table.xlsx
+++ b/data/raw/NM-recognition/tmp/Br_Ib_RT_ID_table.xlsx
@@ -1545,12 +1545,12 @@
   <dimension ref="A1:AQ350"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A259" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A265" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="AN286" activeCellId="0" sqref="AN286"/>
+      <selection pane="bottomLeft" activeCell="T286" activeCellId="0" sqref="T286"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.02"/>
   </cols>

</xml_diff>